<commit_message>
Updated capacity of WB RES
</commit_message>
<xml_diff>
--- a/data/cost/eia_cost_tables.xlsx
+++ b/data/cost/eia_cost_tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5230_ox_ac_uk/Documents/local/OMS/data/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98D07215-EECA-7A4E-BB9E-8070B1D2D8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{98D07215-EECA-7A4E-BB9E-8070B1D2D8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A1474F9-77E5-DD4C-BE91-7B305D71106E}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="960" windowWidth="15640" windowHeight="18400" xr2:uid="{E0A3C9C0-AB34-CD4A-A1E1-FFDBE67E28BA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{E0A3C9C0-AB34-CD4A-A1E1-FFDBE67E28BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Technology</t>
   </si>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23578C1F-AF00-3D47-8FD8-C153579CBA7A}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,10 +859,194 @@
         <v>181.08391851776028</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1175</v>
+      </c>
+      <c r="C13">
+        <v>16.3</v>
+      </c>
+      <c r="D13">
+        <v>4.7</v>
+      </c>
+      <c r="E13">
+        <v>0.13929532193673866</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>181.08391851776028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1175</v>
+      </c>
+      <c r="C14">
+        <v>16.3</v>
+      </c>
+      <c r="D14">
+        <v>4.7</v>
+      </c>
+      <c r="E14">
+        <v>0.13929532193673866</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>181.08391851776028</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1313</v>
+      </c>
+      <c r="C15">
+        <v>15.25</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3676</v>
+      </c>
+      <c r="C16">
+        <v>40.58</v>
+      </c>
+      <c r="D16">
+        <v>4.5</v>
+      </c>
+      <c r="E16">
+        <v>9.2863547957825782E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.13929532193673866</v>
+      </c>
+      <c r="G16">
+        <v>318.83151465520183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>1389</v>
+      </c>
+      <c r="C17">
+        <v>24.8</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1677</v>
+      </c>
+      <c r="C18">
+        <v>35.14</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>1175</v>
+      </c>
+      <c r="C19">
+        <v>16.3</v>
+      </c>
+      <c r="D19">
+        <v>4.7</v>
+      </c>
+      <c r="E19">
+        <v>0.13929532193673866</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>181.08391851776028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
     </row>
   </sheetData>

</xml_diff>